<commit_message>
[Prototype] Add ex_PersonTimeline module
</commit_message>
<xml_diff>
--- a/Prototype/TESTS/GetReferences/PeopleEvents.xlsx
+++ b/Prototype/TESTS/GetReferences/PeopleEvents.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TEST\VSCode\HelloWorld\TESTS\GetReferences\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TEST\VSCode\Prototype\TESTS\GetReferences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC202AA8-BC82-462F-8947-CC8F5553C787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4824D026-90B6-46A4-9C02-337D1EF1BC24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{368C8D5A-6B7F-4890-8AA1-E874F0DCC219}"/>
   </bookViews>
@@ -38,30 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="77">
   <si>
-    <t>ФИО</t>
-  </si>
-  <si>
-    <t>Иванов Иван Иванович</t>
-  </si>
-  <si>
-    <t>Петров Пётр Петрович</t>
-  </si>
-  <si>
-    <t>Сидорова Анна Сергеевна</t>
-  </si>
-  <si>
-    <t>Шевченко Олег Андреевич</t>
-  </si>
-  <si>
-    <t>Отдел</t>
-  </si>
-  <si>
-    <t>Должность</t>
-  </si>
-  <si>
-    <t>Оклад</t>
-  </si>
-  <si>
     <t>IT</t>
   </si>
   <si>
@@ -83,9 +59,6 @@
     <t>QA</t>
   </si>
   <si>
-    <t>Новикова Елена Викторовна</t>
-  </si>
-  <si>
     <t>Finance</t>
   </si>
   <si>
@@ -110,21 +83,9 @@
     <t>3200</t>
   </si>
   <si>
-    <t>ДатаСобытия</t>
-  </si>
-  <si>
-    <t>ТипСобытия</t>
-  </si>
-  <si>
     <t>RecordNo</t>
   </si>
   <si>
-    <t>Повышение</t>
-  </si>
-  <si>
-    <t>Принят</t>
-  </si>
-  <si>
     <t>Sales Rep</t>
   </si>
   <si>
@@ -134,9 +95,6 @@
     <t>Platform</t>
   </si>
   <si>
-    <t>Перевод</t>
-  </si>
-  <si>
     <t>BizDev</t>
   </si>
   <si>
@@ -267,6 +225,48 @@
   </si>
   <si>
     <t>12</t>
+  </si>
+  <si>
+    <t>FIO</t>
+  </si>
+  <si>
+    <t>EventDate</t>
+  </si>
+  <si>
+    <t>EventType</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>Ivanov Ivan Ivanovich</t>
+  </si>
+  <si>
+    <t>Promotion</t>
+  </si>
+  <si>
+    <t>Petrov Pyotr Petrovich</t>
+  </si>
+  <si>
+    <t>Hired</t>
+  </si>
+  <si>
+    <t>Sidorova Anna Sergeevna</t>
+  </si>
+  <si>
+    <t>Shevchenko Oleg Andreevich</t>
+  </si>
+  <si>
+    <t>Transfer</t>
+  </si>
+  <si>
+    <t>Novikova Elena Viktorovna</t>
   </si>
 </sst>
 </file>
@@ -876,12 +876,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8476FCEB-77CB-498F-9487-97259B731F71}" name="TableEvents" displayName="TableEvents" ref="A1:G16" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
   <autoFilter ref="A1:G16" xr:uid="{8476FCEB-77CB-498F-9487-97259B731F71}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{FAADC23F-D7F3-4749-8ECC-9DD1B85C11CA}" name="ФИО" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{F1D6476A-7EC3-428F-AE8D-19EB6A86276D}" name="ДатаСобытия" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{559D4FDC-65CF-4496-B7F0-4A843828BB35}" name="ТипСобытия" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{9A1B1ABD-E1AB-413D-8F0B-1E5A5685CD21}" name="Отдел" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{0475AF35-8E5E-442A-9F12-6652AA5ECFBE}" name="Должность" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{E7E38E6C-7044-4AB9-9214-BA3D732A9537}" name="Оклад" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{FAADC23F-D7F3-4749-8ECC-9DD1B85C11CA}" name="FIO" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{F1D6476A-7EC3-428F-AE8D-19EB6A86276D}" name="EventDate" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{559D4FDC-65CF-4496-B7F0-4A843828BB35}" name="EventType" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{9A1B1ABD-E1AB-413D-8F0B-1E5A5685CD21}" name="Department" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{0475AF35-8E5E-442A-9F12-6652AA5ECFBE}" name="Position" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{E7E38E6C-7044-4AB9-9214-BA3D732A9537}" name="Salary" dataDxfId="1"/>
     <tableColumn id="7" xr3:uid="{15032567-224D-4048-ABCB-285574422F5C}" name="RecordNo" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1208,7 +1208,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1225,370 +1225,370 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="F2" s="3" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="G3" s="8" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>28</v>
+        <v>72</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>4</v>
+        <v>74</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>28</v>
+        <v>72</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>2</v>
+        <v>71</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="8" t="s">
         <v>52</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>15</v>
+        <v>76</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>28</v>
+        <v>72</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>28</v>
+        <v>72</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="E10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="G10" s="8" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>4</v>
+        <v>74</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="G12" s="8" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="F13" s="3" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="D14" s="3" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>15</v>
+        <v>76</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>4</v>
+        <v>74</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>